<commit_message>
Columnas de declaración de esfuerzo.
</commit_message>
<xml_diff>
--- a/Declaracion Esfuerzo.xlsx
+++ b/Declaracion Esfuerzo.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjoven/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f.reyes948\git\201810_01_keuta\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350693A3-9BC0-4FC1-93E9-4DCE9AD54256}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Declaracion" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Nota: De acuerdo al programa del curso cada experimento tiene una nota global (en el ejemplo de abajo es B3) y una nota individual (columna K), esta última depende del esfuerzo de cada miembro (columna J). A ese esfuerzo se llega a partir de una reunión de grupo en donde se revisan las contribuciones de cada miembro para poner en funcionamiento cada uno de los puntos de arquitectura. Las celdas B12 a B20 ejemplifican los puntos para el exp. 1. Si el miembro del equipo contribuyó en ese punto de la arquitectura se marca con X. Luego, a partir de las X, el grupo estima el porcentaje de esfuerzo de cada miembro. 
 Se espera que Uds. suban a github un excel similar a este, en donde enuncien el esfuerzo de cada miembro. A partir de allí y la nota global del experimento, el instructor calculará la nota individual. El máximo valor de la nota individual es 5.</t>
@@ -61,12 +62,33 @@
   </si>
   <si>
     <t>Susan joven</t>
+  </si>
+  <si>
+    <t>Servicios REST para la aplicación</t>
+  </si>
+  <si>
+    <t>Controlador de la aplicación</t>
+  </si>
+  <si>
+    <t>Vista de la aplicación</t>
+  </si>
+  <si>
+    <t>Afiche</t>
+  </si>
+  <si>
+    <t>SAD</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -136,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -152,9 +174,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -165,10 +184,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,170 +475,257 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="202" zoomScaleNormal="202" zoomScalePageLayoutView="202" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="202" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="5" width="14.5" style="11"/>
-    <col min="6" max="6" width="16" style="10" customWidth="1"/>
-    <col min="7" max="7" width="16.1640625" customWidth="1"/>
-    <col min="8" max="8" width="23.6640625" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" customWidth="1"/>
+    <col min="2" max="7" width="14.42578125" style="13"/>
+    <col min="8" max="11" width="14.42578125" style="10"/>
+    <col min="12" max="12" width="16" style="9" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" customWidth="1"/>
+    <col min="14" max="14" width="23.7109375" customWidth="1"/>
+    <col min="17" max="17" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
       <c r="L1" s="15"/>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
-    </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+    </row>
+    <row r="3" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
-    </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+    </row>
+    <row r="4" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="16">
+        <v>1</v>
+      </c>
+      <c r="C4" s="16">
+        <v>2</v>
+      </c>
+      <c r="D4" s="16">
+        <v>3</v>
+      </c>
+      <c r="E4" s="16">
+        <v>4</v>
+      </c>
+      <c r="F4" s="16">
         <v>5</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="G4" s="16">
+        <v>6</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
-    </row>
-    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+    </row>
+    <row r="5" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="6">
         <v>20</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
+      <c r="I5" s="5"/>
+      <c r="L5" s="10"/>
       <c r="M5" s="7"/>
-    </row>
-    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="N5" s="10"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+    </row>
+    <row r="6" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="3">
         <v>20</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-    </row>
-    <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="I6" s="5"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+    </row>
+    <row r="7" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="6">
         <v>20</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-    </row>
-    <row r="8" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I7" s="5"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+    </row>
+    <row r="8" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="6">
         <v>20</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-    </row>
-    <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="I8" s="5"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+    </row>
+    <row r="9" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="3">
         <v>20</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="I9" s="5"/>
+      <c r="P9" s="7"/>
+    </row>
+    <row r="10" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="J10" s="7"/>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="P10" s="7"/>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -624,191 +738,304 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
-    </row>
-    <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+    </row>
+    <row r="12" spans="1:19" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="17">
+        <v>1</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
       <c r="L12" s="7"/>
-    </row>
-    <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+    </row>
+    <row r="13" spans="1:19" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="18">
+        <v>2</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
-    </row>
-    <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+    </row>
+    <row r="14" spans="1:19" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="18">
+        <v>3</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
-    </row>
-    <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="G15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-    </row>
-    <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+    </row>
+    <row r="15" spans="1:19" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
+        <v>4</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="M15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+    </row>
+    <row r="16" spans="1:19" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="18">
+        <v>5</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
-    </row>
-    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="11"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+    </row>
+    <row r="17" spans="1:18" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="18">
+        <v>6</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
-    </row>
-    <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+    </row>
+    <row r="18" spans="1:18" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
       <c r="L18" s="7"/>
-    </row>
-    <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="11"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+    </row>
+    <row r="19" spans="1:18" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
-    </row>
-    <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="11"/>
+      <c r="M19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+    </row>
+    <row r="20" spans="1:18" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
-    </row>
-    <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-    </row>
-    <row r="22" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="11"/>
-    </row>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-    </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="11"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+    </row>
+    <row r="21" spans="1:18" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+    </row>
+    <row r="22" spans="1:18" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+    </row>
+    <row r="23" spans="1:18" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+    </row>
+    <row r="24" spans="1:18" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
       <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="11"/>
-    </row>
-    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="G27" s="11"/>
-      <c r="H27" s="7"/>
-    </row>
-    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="G28" s="7"/>
-      <c r="H28" s="11"/>
-    </row>
-    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-    </row>
-    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-    </row>
-    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="G31" s="11"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="N24" s="7"/>
+    </row>
+    <row r="25" spans="1:18" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+    </row>
+    <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="10"/>
+    </row>
+    <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M27" s="10"/>
+      <c r="N27" s="7"/>
+    </row>
+    <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M28" s="7"/>
+      <c r="N28" s="10"/>
+    </row>
+    <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+    </row>
+    <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+    </row>
+    <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M31" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>